<commit_message>
More cleaning and testing for 1.0.0.
</commit_message>
<xml_diff>
--- a/tests/test_convert/testing_files/main_dir/mwtab_nmr_conversion_directives_compare.xlsx
+++ b/tests/test_convert/testing_files/main_dir/mwtab_nmr_conversion_directives_compare.xlsx
@@ -337,7 +337,7 @@
     <t>*#.exclusion_headers</t>
   </si>
   <si>
-    <t>id,intensity,intensity%type,intensity%units,assignment,assignment%method,entity.id,protocol.id,base_inchi,representative_inchi,isotopic_inchi,peak_description,peak_pattern,proton_count,transient_peak,transient_peak%type</t>
+    <t>id,intensity,intensity%type,intensity%units,assignment,assignment%method,entity.id,protocol.id,base_inchi,representative_inchi,isotopic_inchi,peak_description,peak_pattern,proton_count,transient_peak,transient_peak%type,compound</t>
   </si>
   <si>
     <t>intensity%type</t>
@@ -397,7 +397,7 @@
     <t>*#.optional_headers</t>
   </si>
   <si>
-    <t>assignment%method,base_inchi,representative_inchi,isotopic_inchi,peak_description,peak_pattern,proton_count,transient_peak,transient_peak%type</t>
+    <t>assignment%method,base_inchi,representative_inchi,isotopic_inchi,peak_description,peak_pattern,proton_count,transient_peak,transient_peak%type,compound</t>
   </si>
   <si>
     <t>measurement</t>

</xml_diff>